<commit_message>
fix script alerta eca
</commit_message>
<xml_diff>
--- a/app/data/tabla_alertas.xlsx
+++ b/app/data/tabla_alertas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eigonzalez/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAADE69E-C60E-3A45-90CB-B810CA52DF9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{652A8423-CF61-AD4E-8218-95B4EE9A5765}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="1800" windowWidth="28040" windowHeight="17440" xr2:uid="{0857D821-8A5B-1745-B4C7-2175F0D1A14D}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19500" xr2:uid="{CC93169C-F928-354C-98A0-4862322C87BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,93 +36,57 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="29">
-  <si>
-    <t>Grados días Acumulados Opt</t>
-  </si>
-  <si>
-    <t>T base (Parámetro °C)</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
+  <si>
+    <t>Cultivo</t>
+  </si>
+  <si>
+    <t>Fase</t>
   </si>
   <si>
     <t>Temperatura crítica mínima</t>
   </si>
   <si>
-    <t>T° mínima de crecimiento</t>
-  </si>
-  <si>
-    <t>Rango T° Mínimo Óptimo</t>
-  </si>
-  <si>
-    <t>Rango T° Máximo Óptimo</t>
-  </si>
-  <si>
-    <t>T° máxima de crecimiento</t>
+    <t>Vid</t>
   </si>
   <si>
     <t>Receso invernal</t>
   </si>
   <si>
-    <t>-10 °C</t>
-  </si>
-  <si>
-    <t>brotación</t>
-  </si>
-  <si>
-    <t>-2°C</t>
-  </si>
-  <si>
-    <t>10°C</t>
-  </si>
-  <si>
-    <t>18°C</t>
-  </si>
-  <si>
-    <t>25°C</t>
-  </si>
-  <si>
-    <t>35°C - 40°C</t>
-  </si>
-  <si>
-    <t>foliación</t>
-  </si>
-  <si>
-    <t>floración</t>
-  </si>
-  <si>
-    <t>0°C</t>
-  </si>
-  <si>
-    <t>20°C</t>
-  </si>
-  <si>
-    <t>28°C</t>
-  </si>
-  <si>
-    <t>fructificación</t>
-  </si>
-  <si>
-    <t>15°C</t>
-  </si>
-  <si>
-    <t>30°C</t>
-  </si>
-  <si>
-    <t>envero o pinta (coloración fruto)</t>
-  </si>
-  <si>
-    <t>maduración</t>
-  </si>
-  <si>
-    <t>cosecha</t>
-  </si>
-  <si>
-    <t>Vid</t>
-  </si>
-  <si>
-    <t>Cultivo</t>
-  </si>
-  <si>
-    <t>Fase</t>
+    <t>GDA Optimo</t>
+  </si>
+  <si>
+    <t>Temperatura mínima de crecimiento</t>
+  </si>
+  <si>
+    <t>Rango Temperatura Mínimo Óptimo</t>
+  </si>
+  <si>
+    <t>Rango Temperatura Máximo Óptimo</t>
+  </si>
+  <si>
+    <t>Temperatura máxima de crecimiento</t>
+  </si>
+  <si>
+    <t>Floración</t>
+  </si>
+  <si>
+    <t>Brotación</t>
+  </si>
+  <si>
+    <t>Foliación</t>
+  </si>
+  <si>
+    <t>Fructificación</t>
+  </si>
+  <si>
+    <t>Envero o Pinta</t>
+  </si>
+  <si>
+    <t>Maduración</t>
+  </si>
+  <si>
+    <t>Cosecha</t>
   </si>
 </sst>
 </file>
@@ -493,270 +457,242 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81E8784F-48E9-824A-A245-15AB307F780A}">
-  <dimension ref="A1:I9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7829D405-C72A-3441-AFBA-BDC2BA822515}">
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:C8"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>28</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
+      <c r="B2" t="s">
         <v>4</v>
-      </c>
-      <c r="H1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
       <c r="D2">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C3">
         <v>33</v>
       </c>
       <c r="D3">
+        <v>-2</v>
+      </c>
+      <c r="E3">
         <v>10</v>
       </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="F3">
+        <v>18</v>
+      </c>
+      <c r="G3">
+        <v>25</v>
+      </c>
+      <c r="H3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>12</v>
-      </c>
-      <c r="H3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" t="s">
-        <v>15</v>
       </c>
       <c r="C4">
         <v>69</v>
       </c>
       <c r="D4">
+        <v>-2</v>
+      </c>
+      <c r="E4">
         <v>10</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4">
+        <v>18</v>
+      </c>
+      <c r="G4">
+        <v>25</v>
+      </c>
+      <c r="H4">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
         <v>10</v>
-      </c>
-      <c r="F4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" t="s">
-        <v>13</v>
-      </c>
-      <c r="I4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" t="s">
-        <v>16</v>
       </c>
       <c r="C5">
         <v>283</v>
       </c>
       <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
         <v>10</v>
       </c>
-      <c r="E5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H5" t="s">
-        <v>19</v>
-      </c>
-      <c r="I5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F5">
+        <v>20</v>
+      </c>
+      <c r="G5">
+        <v>28</v>
+      </c>
+      <c r="H5">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C6">
         <v>374</v>
       </c>
       <c r="D6">
-        <v>10</v>
-      </c>
-      <c r="E6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G6" t="s">
-        <v>13</v>
-      </c>
-      <c r="H6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>15</v>
+      </c>
+      <c r="F6">
+        <v>25</v>
+      </c>
+      <c r="G6">
+        <v>30</v>
+      </c>
+      <c r="H6">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" t="s">
-        <v>23</v>
       </c>
       <c r="C7">
         <v>980</v>
       </c>
       <c r="D7">
-        <v>10</v>
-      </c>
-      <c r="E7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H7" t="s">
-        <v>22</v>
-      </c>
-      <c r="I7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+      <c r="E7">
+        <v>18</v>
+      </c>
+      <c r="F7">
+        <v>25</v>
+      </c>
+      <c r="G7">
+        <v>30</v>
+      </c>
+      <c r="H7">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="D8">
-        <v>10</v>
-      </c>
-      <c r="E8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" t="s">
-        <v>12</v>
-      </c>
-      <c r="G8" t="s">
-        <v>13</v>
-      </c>
-      <c r="H8" t="s">
-        <v>22</v>
-      </c>
-      <c r="I8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+      <c r="E8">
+        <v>18</v>
+      </c>
+      <c r="F8">
+        <v>25</v>
+      </c>
+      <c r="G8">
+        <v>30</v>
+      </c>
+      <c r="H8">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="C9">
         <v>1478</v>
       </c>
       <c r="D9">
-        <v>10</v>
-      </c>
-      <c r="E9" t="s">
-        <v>13</v>
-      </c>
-      <c r="F9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G9" t="s">
-        <v>13</v>
-      </c>
-      <c r="H9" t="s">
-        <v>22</v>
-      </c>
-      <c r="I9" t="s">
-        <v>14</v>
+        <v>25</v>
+      </c>
+      <c r="E9">
+        <v>20</v>
+      </c>
+      <c r="F9">
+        <v>25</v>
+      </c>
+      <c r="G9">
+        <v>30</v>
+      </c>
+      <c r="H9">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>